<commit_message>
Edit for download Shop Address
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/BB_Shop_Address.xlsx
+++ b/application/controllers/excel-templates/BB_Shop_Address.xlsx
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
-  <si>
-    <t xml:space="preserve">CP ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">Contact Person</t>
   </si>
@@ -55,15 +52,6 @@
     <t xml:space="preserve">TIN Number</t>
   </si>
   <si>
-    <t xml:space="preserve">Active</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create_Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{data:cp_id}</t>
-  </si>
-  <si>
     <t xml:space="preserve">{data:contact_person}</t>
   </si>
   <si>
@@ -89,9 +77,6 @@
   </si>
   <si>
     <t xml:space="preserve">{data:tin_number}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{data:active}</t>
   </si>
 </sst>
 </file>
@@ -213,24 +198,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="1:2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.7857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.1326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9642857142857"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="46.5714285714286"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.484693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="34.5561224489796"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.7295918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.5561224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.030612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.0765306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -264,63 +250,50 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="H2" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="{data:contact_person}"/>
-    <hyperlink ref="C2" r:id="rId2" display="{data:contact_email}"/>
-    <hyperlink ref="D2" r:id="rId3" display="{data:shop_address_line1}"/>
-    <hyperlink ref="F2" r:id="rId4" display="{data:shop_address_city}"/>
-    <hyperlink ref="G2" r:id="rId5" display="{data:shop_address_state}"/>
-    <hyperlink ref="H2" r:id="rId6" display="{data:shop_address_pincode}"/>
-    <hyperlink ref="J2" r:id="rId7" display="{data:phone_number}"/>
-    <hyperlink ref="K2" r:id="rId8" display="{data:tin_number}"/>
-    <hyperlink ref="L2" r:id="rId9" display="{data:active}"/>
+    <hyperlink ref="A2" r:id="rId1" display="{data:contact_person}"/>
+    <hyperlink ref="B2" r:id="rId2" display="{data:contact_email}"/>
+    <hyperlink ref="C2" r:id="rId3" display="{data:shop_address_line1}"/>
+    <hyperlink ref="E2" r:id="rId4" display="{data:shop_address_city}"/>
+    <hyperlink ref="F2" r:id="rId5" display="{data:shop_address_state}"/>
+    <hyperlink ref="G2" r:id="rId6" display="{data:shop_address_pincode}"/>
+    <hyperlink ref="I2" r:id="rId7" display="{data:phone_number}"/>
+    <hyperlink ref="J2" r:id="rId8" display="{data:tin_number}"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>